<commit_message>
fix QForum Validate Bug and add htmldecode
</commit_message>
<xml_diff>
--- a/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
+++ b/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="14805" windowHeight="7965"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="getBoardList" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
-    <sheet name="工作表3" sheetId="3" r:id="rId3"/>
+    <sheet name="getPostId" sheetId="2" r:id="rId2"/>
+    <sheet name="newPost" sheetId="3" r:id="rId3"/>
+    <sheet name="newComment" sheetId="4" r:id="rId4"/>
+    <sheet name="getPostDetails" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="129">
   <si>
     <t>scenario</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -132,9 +134,6 @@
   <si>
     <t>沒有建立資料</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
   </si>
   <si>
     <t>ok</t>
@@ -247,41 +246,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1106018&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
-  </si>
-  <si>
     <t>compant = Qisda
 empno=1106018</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-    "ResultCode": "1",
-    "token_valid": 1516868949,
-    "Message": "",
-    "Content": {
-        "board_list": [
-            {
-                "board_type_id": 3,
-                "board_type_name": "視聽劇場",
-                "board_id": 7,
-                "board_name": "公司每季電影討論版",
-                "board_manager": "",
-                "board_status": "Y",
-                "board_public_type": "1"
-            },
-            {
-                "board_type_id": 2,
-                "board_type_name": "活動中心",
-                "board_id": 6,
-                "board_name": "烏克莉莉社",
-                "board_manager": "",
-                "board_status": "Y",
-                "board_public_type": "2"
-            }
-        ]
-    }
-}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -327,12 +293,568 @@
     <t>company = BenQAA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607280&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;/LayoutHeader&gt;"&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;/LayoutHeader&gt;"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;123456&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;AAAAAAAAAAAAAAAAAAA&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": "bb32d3c0fcbf11e7a72b15b366a00a45"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emp_no  =  1607279</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": "f77ee810fcbf11e79cc8918b657b8ae5"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1106018&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;AAAA&lt;/emp_no&gt;&lt;board_id&gt;4&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試新貼文&lt;/post_title&gt;&lt;content&gt;測試內文&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;123456&lt;/emp_no&gt;&lt;board_id&gt;4&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試新貼文&lt;/post_title&gt;&lt;content&gt;測試內文&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;board_id&gt;4&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試新貼文&lt;/post_title&gt;&lt;content&gt;測試內文&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;board_id&gt;4&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試新貼文&lt;/post_title&gt;&lt;content&gt;測試內文&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>不存在的board_id
+emp_no  =  1607279
+board_id = 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;14&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試新貼文&lt;/post_title&gt;&lt;content&gt;測試內文&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047904",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沒有權限的board_id
+empno=1607279</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1106018&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試新貼文&lt;/post_title&gt;&lt;content&gt;測試內文&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沒有權限的board_id
+board_id = 13
+empno=1106018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047904",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "Message": "Success",
+    "token_valid": 1516868949,
+    "Content": {
+        "post_id": 0
+    }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;0407731&lt;/emp_no&gt;&lt;board_id&gt;12&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;post_title&gt;測試有圖片的內文&lt;/post_title&gt;&lt;content&gt;&amp;lt;h2&amp;gt;Essential things to think about before starting a blog&amp;lt;/h2&amp;gt;&amp;lt;figure class=&amp;quot;image illustration&amp;quot;&amp;gt;&amp;lt;img alt=&amp;quot;Blog&amp;quot; src=&amp;quot;/assets/images/bg/spoons.jpg&amp;quot;&amp;gt;&amp;lt;figcaption&amp;gt;It takes several ingredients to create a delicious blog.&amp;lt;/figcaption&amp;gt;&amp;lt;/figure&amp;gt;&amp;lt;p&amp;gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &amp;lt;strong&amp;gt;my full-time job&amp;lt;/strong&amp;gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;I am now a &amp;lt;strong&amp;gt;full-time blogger&amp;lt;/strong&amp;gt; and the curator of the &amp;lt;a href=&amp;quot;https://ckeditor.com/ckeditor-4/#&amp;quot;&amp;gt;Simply delicious newsletter&amp;lt;/a&amp;gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;If you are tempted by the idea of creating your own blog, please think about the following:&amp;lt;/p&amp;gt;&amp;lt;ul&amp;gt;&amp;lt;li&amp;gt;Your story (what do you want to tell your audience)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your audience (who do you write for)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your blog name and design&amp;lt;/li&amp;gt;&amp;lt;/ul&amp;gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試沒有圖片的內文
+empno=1607279</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試有圖片的內文
+empno=0407731</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047902",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;0407731&lt;/emp_no&gt;&lt;board_id&gt;12&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;post_title&gt;測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文測試有圖片的內文&lt;/post_title&gt;&lt;content&gt;&amp;lt;h2&amp;gt;Essential things to think about before starting a blog&amp;lt;/h2&amp;gt;&amp;lt;figure class=&amp;quot;image illustration&amp;quot;&amp;gt;&amp;lt;img alt=&amp;quot;Blog&amp;quot; src=&amp;quot;/assets/images/bg/spoons.jpg&amp;quot;&amp;gt;&amp;lt;figcaption&amp;gt;It takes several ingredients to create a delicious blog.&amp;lt;/figcaption&amp;gt;&amp;lt;/figure&amp;gt;&amp;lt;p&amp;gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &amp;lt;strong&amp;gt;my full-time job&amp;lt;/strong&amp;gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;I am now a &amp;lt;strong&amp;gt;full-time blogger&amp;lt;/strong&amp;gt; and the curator of the &amp;lt;a href=&amp;quot;https://ckeditor.com/ckeditor-4/#&amp;quot;&amp;gt;Simply delicious newsletter&amp;lt;/a&amp;gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;If you are tempted by the idea of creating your own blog, please think about the following:&amp;lt;/p&amp;gt;&amp;lt;ul&amp;gt;&amp;lt;li&amp;gt;Your story (what do you want to tell your audience)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your audience (who do you write for)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your blog name and design&amp;lt;/li&amp;gt;&amp;lt;/ul&amp;gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"strXml":"&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;我是2樓HI~~&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;我是2樓HI~~&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_id未瑱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047916</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047903",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047903</t>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047908",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047908</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;&lt;/post_id&gt;&lt;content&gt;我是2樓HI~~&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>conetne未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047905</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;aaa&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;aaa&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;YSYSYS123######&lt;/post_id&gt;&lt;content&gt;aaa&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_id格式錯誤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047905</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expected result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少post_id節點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少ocntent節點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;aaa&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;aaa&lt;/emp_no&gt;&lt;content&gt;aaa&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;aaa&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047904</t>
+  </si>
+  <si>
+    <t>047904</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047904",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沒有該討論版的權限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不存在的pos_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試有圖片的評論</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試沒有圖片的評論</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;post_title&gt;測試沒有圖片的內文&lt;/post_title&gt;&lt;content&gt;&amp;lt;h2&amp;gt;Essential things to think about before starting a blog&amp;lt;/h2&amp;gt;&amp;lt;figure class=&amp;quot;image illustration&amp;quot;&amp;gt;&amp;lt;img alt=&amp;quot;Blog&amp;quot; src=&amp;quot;/assets/images/bg/spoons.jpg&amp;quot;&amp;gt;&amp;lt;figcaption&amp;gt;It takes several ingredients to create a delicious blog.&amp;lt;/figcaption&amp;gt;&amp;lt;/figure&amp;gt;&amp;lt;p&amp;gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &amp;lt;strong&amp;gt;my full-time job&amp;lt;/strong&amp;gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;I am now a &amp;lt;strong&amp;gt;full-time blogger&amp;lt;/strong&amp;gt; and the curator of the &amp;lt;a href=&amp;quot;https://ckeditor.com/ckeditor-4/#&amp;quot;&amp;gt;Simply delicious newsletter&amp;lt;/a&amp;gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;If you are tempted by the idea of creating your own blog, please think about the following:&amp;lt;/p&amp;gt;&amp;lt;ul&amp;gt;&amp;lt;li&amp;gt;Your story (what do you want to tell your audience)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your audience (who do you write for)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your blog name and design&amp;lt;/li&amp;gt;&amp;lt;/ul&amp;gt;&lt;/content&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;&amp;lt;h2&amp;gt;Essential things to think about before starting a blog&amp;lt;/h2&amp;gt;&amp;lt;figure class=&amp;quot;image illustration&amp;quot;&amp;gt;&amp;lt;img alt=&amp;quot;Blog&amp;quot; src=&amp;quot;/assets/images/bg/spoons.jpg&amp;quot;&amp;gt;&amp;lt;figcaption&amp;gt;It takes several ingredients to create a delicious blog.&amp;lt;/figcaption&amp;gt;&amp;lt;/figure&amp;gt;&amp;lt;p&amp;gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &amp;lt;strong&amp;gt;my full-time job&amp;lt;/strong&amp;gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;I am now a &amp;lt;strong&amp;gt;full-time blogger&amp;lt;/strong&amp;gt; and the curator of the &amp;lt;a href=&amp;quot;https://ckeditor.com/ckeditor-4/#&amp;quot;&amp;gt;Simply delicious newsletter&amp;lt;/a&amp;gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;If you are tempted by the idea of creating your own blog, please think about the following:&amp;lt;/p&amp;gt;&amp;lt;ul&amp;gt;&amp;lt;li&amp;gt;Your story (what do you want to tell your audience)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your audience (who do you write for)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your blog name and design&amp;lt;/li&amp;gt;&amp;lt;/ul&amp;gt;&lt;/content&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;&amp;lt;h2&amp;gt;Essential things to think about before starting a blog&amp;lt;/h2&amp;gt;&amp;lt;figure class=&amp;quot;image illustration&amp;quot;&amp;gt;&amp;lt;img alt=&amp;quot;Blog&amp;quot; src=&amp;quot;/assets/images/bg/spoons.jpg&amp;quot;&amp;gt;&amp;lt;figcaption&amp;gt;It takes several ingredients to create a delicious blog.&amp;lt;/figcaption&amp;gt;&amp;lt;/figure&amp;gt;&amp;lt;p&amp;gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &amp;lt;strong&amp;gt;my full-time job&amp;lt;/strong&amp;gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;I am now a &amp;lt;strong&amp;gt;full-time blogger&amp;lt;/strong&amp;gt; and the curator of the &amp;lt;a href=&amp;quot;https://ckeditor.com/ckeditor-4/#&amp;quot;&amp;gt;Simply delicious newsletter&amp;lt;/a&amp;gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&amp;lt;/p&amp;gt;&amp;lt;p&amp;gt;If you are tempted by the idea of creating your own blog, please think about the following:&amp;lt;/p&amp;gt;&amp;lt;ul&amp;gt;&amp;lt;li&amp;gt;Your story (what do you want to tell your audience)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your audience (who do you write for)&amp;lt;/li&amp;gt;&amp;lt;li&amp;gt;Your blog name and design&amp;lt;/li&amp;gt;&amp;lt;/ul&amp;gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": {
+        "comment_id": 3
+    }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": {
+        "comment_id": 4
+    }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"strXml":"&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;1&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047916",
+    "token_valid": 1516868949,{
+    "ResultCode": "047916",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"strXml":"&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;board_id&gt;1&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board_id未瑱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post_id未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;1&lt;/board_id&gt;&lt;post_id&gt;&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "ResultCode": "047908",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;123456&lt;/emp_no&gt;&lt;board_id&gt;1&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;AAA&lt;/emp_no&gt;&lt;board_id&gt;1&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;AAA&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;AAA&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少board_id節點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;AAA&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047903",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少reply_from_seq節點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺少reply_to_seq節點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;12&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reply_from_seq &gt; reply_to_seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047905",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帳號沒有討論版權限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607282&lt;/emp_no&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": {
+        "board_list": [
+            {
+                "board_type_id": 3,
+                "board_type_name": "視聽劇場",
+                "board_id": 7,
+                "board_name": "公司每季電影討論版",
+                "board_manager": "",
+                "board_status": "N",
+                "board_public_type": "1"
+            },
+            {
+                "board_type_id": 2,
+                "board_type_name": "活動中心",
+                "board_id": 6,
+                "board_name": "烏克莉莉社",
+                "board_manager": "",
+                "board_status": "Y",
+                "board_public_type": "2"
+            }
+        ]
+    }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047904",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1106018&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;12&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>該篇post不存在該board</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1106018&lt;/emp_no&gt;&lt;board_id&gt;14&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": {
+        "board_id": 13,
+        "board_name": "RM",
+        "board_status": "Y",
+        "post_id": "bb2cbbc0eb8411e7b4f300016cd4175c",
+        "post_title": "測試沒有圖片的內文",
+        "post_content": "&lt;h2&gt;Essential things to think about before starting a blog&lt;/h2&gt;&lt;figure class=\"image illustration\"&gt;&lt;img alt=\"Blog\" src=\"/assets/images/bg/spoons.jpg\"&gt;&lt;figcaption&gt;It takes several ingredients to create a delicious blog.&lt;/figcaption&gt;&lt;/figure&gt;&lt;p&gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &lt;strong&gt;my full-time job&lt;/strong&gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&lt;/p&gt;&lt;p&gt;I am now a &lt;strong&gt;full-time blogger&lt;/strong&gt; and the curator of the &lt;a href=\"https://ckeditor.com/ckeditor-4/#\"&gt;Simply delicious newsletter&lt;/a&gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&lt;/p&gt;&lt;p&gt;If you are tempted by the idea of creating your own blog, please think about the following:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Your story (what do you want to tell your audience)&lt;/li&gt;&lt;li&gt;Your audience (who do you write for)&lt;/li&gt;&lt;li&gt;Your blog name and design&lt;/li&gt;&lt;/ul&gt;",
+        "post_creator": "Cleo.W.Chan",
+        "post_create_time": "2018-01-19 06:05:27",
+        "post_update_time": null,
+        "post_delete_time": null,
+        "reply_list": [
+            {
+                "comment_id": 1,
+                "sequence_id": 0,
+                "reply_content": "&lt;h2&gt;Essential things to think about before starting a blog&lt;/h2&gt;&lt;figure class=\"image illustration\"&gt;&lt;img alt=\"Blog\" src=\"/assets/images/bg/spoons.jpg\"&gt;&lt;figcaption&gt;It takes several ingredients to create a delicious blog.&lt;/figcaption&gt;&lt;/figure&gt;&lt;p&gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &lt;strong&gt;my full-time job&lt;/strong&gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&lt;/p&gt;&lt;p&gt;I am now a &lt;strong&gt;full-time blogger&lt;/strong&gt; and the curator of the &lt;a href=\"https://ckeditor.com/ckeditor-4/#\"&gt;Simply delicious newsletter&lt;/a&gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&lt;/p&gt;&lt;p&gt;If you are tempted by the idea of creating your own blog, please think about the following:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Your story (what do you want to tell your audience)&lt;/li&gt;&lt;li&gt;Your audience (who do you write for)&lt;/li&gt;&lt;li&gt;Your blog name and design&lt;/li&gt;&lt;/ul&gt;",
+                "reply_user": "Cleo.W.Chan",
+                "updated_user": null,
+                "reply_create_time": "2018-01-19 07:05:47",
+                "reply_update_time": null,
+                "reply_delete_time": null
+            },
+            {
+                "comment_id": 3,
+                "sequence_id": 1,
+                "reply_content": "&lt;h2&gt;Essential things to think about before starting a blog&lt;/h2&gt;&lt;figure class=\"image illustration\"&gt;&lt;img alt=\"Blog\" src=\"/assets/images/bg/spoons.jpg\"&gt;&lt;figcaption&gt;It takes several ingredients to create a delicious blog.&lt;/figcaption&gt;&lt;/figure&gt;&lt;p&gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &lt;strong&gt;my full-time job&lt;/strong&gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&lt;/p&gt;&lt;p&gt;I am now a &lt;strong&gt;full-time blogger&lt;/strong&gt; and the curator of the &lt;a href=\"https://ckeditor.com/ckeditor-4/#\"&gt;Simply delicious newsletter&lt;/a&gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&lt;/p&gt;&lt;p&gt;If you are tempted by the idea of creating your own blog, please think about the following:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Your story (what do you want to tell your audience)&lt;/li&gt;&lt;li&gt;Your audience (who do you write for)&lt;/li&gt;&lt;li&gt;Your blog name and design&lt;/li&gt;&lt;/ul&gt;",
+                "reply_user": "Cleo.W.Chan",
+                "updated_user": null,
+                "reply_create_time": "2018-01-19 07:14:56",
+                "reply_update_time": null,
+                "reply_delete_time": null
+            },
+            {
+                "comment_id": 4,
+                "sequence_id": 2,
+                "reply_content": "&lt;h2&gt;Essential things to think about before starting a blog&lt;/h2&gt;&lt;figure class=\"image illustration\"&gt;&lt;img alt=\"Blog\" src=\"/assets/images/bg/spoons.jpg\"&gt;&lt;figcaption&gt;It takes several ingredients to create a delicious blog.&lt;/figcaption&gt;&lt;/figure&gt;&lt;p&gt;It has been exactly 3 years since I wrote my first blog series entitled “Flavorful Tuscany”, but starting it was definitely not easy. Back then, I didn’t know much about blogging, let alone think that one day it could become &lt;strong&gt;my full-time job&lt;/strong&gt;. Even though I had many recipes and food-related stories to tell, it never crossed my mind that I could be sharing them with the whole world&lt;/p&gt;&lt;p&gt;I am now a &lt;strong&gt;full-time blogger&lt;/strong&gt; and the curator of the &lt;a href=\"https://ckeditor.com/ckeditor-4/#\"&gt;Simply delicious newsletter&lt;/a&gt;, sharing stories about travelling and cooking, as well as tips on how to run a successful blog.&lt;/p&gt;&lt;p&gt;If you are tempted by the idea of creating your own blog, please think about the following:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Your story (what do you want to tell your audience)&lt;/li&gt;&lt;li&gt;Your audience (who do you write for)&lt;/li&gt;&lt;li&gt;Your blog name and design&lt;/li&gt;&lt;/ul&gt;",
+                "reply_user": "Cleo.W.Chan",
+                "updated_user": null,
+                "reply_create_time": "2018-01-19 07:15:58",
+                "reply_update_time": null,
+                "reply_delete_time": null
+            }
+        ]
+    }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取得有權限的討論版內容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +874,27 @@
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -375,11 +918,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -683,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.25" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -785,49 +1348,49 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="384.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -842,12 +1405,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="A8:C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -855,12 +1541,832 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="114" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="26.625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="5"/>
+    <col min="4" max="16384" width="26.625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="9"/>
+    <col min="2" max="2" width="31.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="25.375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="33.375" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Test Case of deletePost
</commit_message>
<xml_diff>
--- a/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
+++ b/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="getBoardList" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="newPost" sheetId="3" r:id="rId3"/>
     <sheet name="newComment" sheetId="4" r:id="rId4"/>
     <sheet name="getPostDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="deletePost" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="148">
   <si>
     <t>scenario</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -849,12 +850,95 @@
   <si>
     <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;board_id&gt;13&lt;/board_id&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;reply_from_seq&gt;1&lt;/reply_from_seq&gt;&lt;reply_to_seq&gt;10&lt;/reply_to_seq&gt;&lt;/LayoutHeader&gt;</t>
   </si>
+  <si>
+    <t>刪除不存在的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除自己的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除已經刪除過的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沒有此討論版的權限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功刪除，status=N,deleted_at=now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回應成功但不更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;post_id&gt;cc2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1205092&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有討論版權限，刪除不是自己建立的貼文，而且不是管理者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047906",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;259939e0001711e88812cd6efd8cdedb&lt;/post_id&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>有討論版權限，管理者刪除不是自己的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功刪除，status=N,deleted_at=now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;0407731&lt;/emp_no&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>deleted_at 維持一樣</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;02b156f0ff7b11e792fb2dc62cd11aaa&lt;/post_id&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -897,6 +981,12 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -918,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -943,6 +1033,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1547,7 +1638,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="41.875" style="2" customWidth="1"/>
@@ -1584,7 +1675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="114" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1598,7 +1689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1612,7 +1703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1640,7 +1731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1666,7 +1757,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -1680,7 +1771,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="370.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1694,7 +1785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="399" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1758,7 +1849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +2050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="370.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>90</v>
       </c>
@@ -1970,7 +2061,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="399" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>89</v>
       </c>
@@ -1991,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2370,4 +2461,145 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.75" style="3" customWidth="1"/>
+    <col min="2" max="5" width="13.625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="114" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="3">
+        <v>47904</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="114" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="3">
+        <v>47904</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="114" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="10">
+        <v>47906</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add modifyPost API & Test Case
</commit_message>
<xml_diff>
--- a/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
+++ b/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="getBoardList" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="newComment" sheetId="4" r:id="rId4"/>
     <sheet name="getPostDetails" sheetId="5" r:id="rId5"/>
     <sheet name="deletePost" sheetId="6" r:id="rId6"/>
+    <sheet name="modifyPost" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="163">
   <si>
     <t>scenario</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -932,6 +933,70 @@
   </si>
   <si>
     <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;02b156f0ff7b11e792fb2dc62cd11aaa&lt;/post_id&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>修改別人的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;post_title&gt;災害發生之應變辦法A&lt;/post_title&gt;&lt;content&gt;應該是就近前往避難場所&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改貼文，attach移除1post2,新增test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1516868949,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;0407731&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;post_title&gt;災害發生之應變辦法A&lt;/post_title&gt;&lt;content&gt;應該是就近前往避難場所&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>帶入與原始相同file_list，attach不異動</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;0407731&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;post_title&gt;災害發生之應變辦法ABC&lt;/post_title&gt;&lt;content&gt;應該是就近前往避難場所&lt;/content&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;0407731&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;post_id&gt;bb2cbbc0eb8411e7b4f300016cd4176c&lt;/post_id&gt;&lt;post_title&gt;災害發生之應變辦法A&lt;/post_title&gt;&lt;content&gt;應該是就近前往避難場所&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/post2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未帶入file_list,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attach全部刪除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attach不異動</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> post2 deleted_at有值，新增test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2467,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2602,4 +2667,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="21.375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="21.375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="171" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="3">
+        <v>47906</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="171" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="114" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="171" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case update ,add modifyComment and deleteComment
</commit_message>
<xml_diff>
--- a/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
+++ b/PlatformDoc/QForum/TestCase/QForum_TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="getBoardList" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="getPostDetails" sheetId="5" r:id="rId5"/>
     <sheet name="deletePost" sheetId="6" r:id="rId6"/>
     <sheet name="modifyPost" sheetId="7" r:id="rId7"/>
+    <sheet name="modifyComment" sheetId="8" r:id="rId8"/>
+    <sheet name="deleteComment" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="281">
   <si>
     <t>scenario</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -996,6 +998,605 @@
   </si>
   <si>
     <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emp_no未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>source未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_id未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出現兩次以上的emp_no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出現兩次以上的source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出現兩次以上的comment_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出現兩次以上的content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出現兩次以上的file_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emp_no 不為數字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_id不為數字</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改content，新增單一檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改content，新增多筆檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改content，將A檔案換成B檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改content，原先有AB檔案,刪除A,新增C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>貼文關閉中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>評論關閉中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改content，刪除所有檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047903，必填欄位缺失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取第一個emp_no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取第一個source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取第一個comment_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取第一個content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取第一個file_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047904，沒有該討論版權限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改不是自己建立的評論</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047911，討論版已關閉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047910，貼文已關閉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047912，回應已刪除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047906，不能修改他人回應</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qp_comment.content被修改，updated_user,updated_at改為修改時間
+qp_attach，
+1.A檔案deleted_at,寫入現在時間
+2.新增一B檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qp_comment
+1.content被修改
+2.updated_user,updated_at改為修改時間
+qp_attach
+1.新增多筆檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qp_comment
+1.content被修改
+2.updated_user,updated_at改為修改時間
+qp_attach
+1.新增一筆檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qp_comment
+1.content被修改
+2.updated_user,updated_at改為修改時間
+qp_attach
+1.A檔案deleted_at,寫入現在時間
+2.B檔案維持不動
+2.新增一C檔案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qp_comment
+1.content被修改
+2.updated_user,updated_at改為修改時間
+qp_attach
+1.修改所有檔案deleted_at為現在時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047905，欄位格式錯誤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047903",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>source節點不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;&lt;/source&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>source來源專案不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047913",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047913，專案來源不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;post_id&gt;aa2cbbc0eb8411e7b4f300016cd4175c&lt;/post_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_id節點不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;&lt;/comment_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_id格式錯誤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047905",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;AAAAA&lt;/comment_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment_id不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047906",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;123456&lt;/comment_id&gt;&lt;content&gt;test test&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>047906，不能修改其他人的回應</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content節點不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/comment1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>有file_list,但file未填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有fileList節點，但沒有file節點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;comment_id&gt;222&lt;/comment_id&gt;&lt;content&gt;&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;AAA&lt;/content&gt;&lt;content&gt;BBB&lt;/content&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}
+資料庫被修改成AAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;BBB&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}
+qp_comment.content被修改成BBB，qp_attach新增一筆test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047905",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;AAA&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;31&lt;/comment_id&gt;&lt;content&gt;BBB&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;AAAAA&lt;/comment_id&gt;&lt;content&gt;BBB&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test1.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/board_id/post_id/test2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用者沒有討論版權限: 開放的公司不符合
+=&gt;將board_company改為開放給Qisda</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;不好意思，請問社長的信箱&lt;/content&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047904",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用者沒有討論版權限: 討論版public_type=3,但user_board無資料
+=&gt;將user從qp_user中移除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;4&lt;/comment_id&gt;&lt;content&gt;Hello&lt;/content&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;Hello&lt;/content&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047911",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>討論版關閉中 
+=&gt;將討論版status設成N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047910",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047912",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;Hello&lt;/content&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;請問社長信箱&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;請問社長信箱&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;請問社長信箱&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/comment_40-aaa.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-2.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}
+commint_40.jpb移除，新增comment_40-aaa.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;請問社長信箱&lt;/content&gt;&lt;file_list&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-1.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-2.jpg&lt;/file&gt;&lt;file&gt;http://XXXX/forum/5/5976779004c211e8bc59a9fefefabbce/commint_40-3.jpg&lt;/file&gt;&lt;/file_list&gt;&lt;/LayoutHeader&gt;</t>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "1",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}
+comment_40-aaa移除,新增commint_40-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;content&gt;請問社長信箱&lt;/content&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emp_no節點不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;aaa&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appdensdev&lt;/source&gt;&lt;comment_id&gt;&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;AAA&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;AAA&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除不是自己的comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1607279&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047906，不能修改其他人的回應</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>討論版關閉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>貼文關閉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment已被刪除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;LayoutHeader&gt;&lt;emp_no&gt;1609009&lt;/emp_no&gt;&lt;source&gt;appensdev&lt;/source&gt;&lt;comment_id&gt;40&lt;/comment_id&gt;&lt;/LayoutHeader&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047911",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047911,討論版已關閉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047910,貼文已關閉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除自己的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>貼文成功刪除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "ResultCode": "047912",
+    "token_valid": 1517555999,
+    "Message": "",
+    "Content": ""
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>047912,貼文已刪除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1073,7 +1674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1099,6 +1700,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -2673,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2772,4 +3379,830 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="27.375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="27.375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="114" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="114" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="185.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="199.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="185.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.5" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="99" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>